<commit_message>
Fixed initial commit BD Tesis User postgres
</commit_message>
<xml_diff>
--- a/laravel/storage/archivos/archivodatos.xlsx
+++ b/laravel/storage/archivos/archivodatos.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>email</t>
   </si>
@@ -73,13 +73,19 @@
   </si>
   <si>
     <t>nilton8hoyos8@gmail.com</t>
+  </si>
+  <si>
+    <t>Paula</t>
+  </si>
+  <si>
+    <t>paula_@hotmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -94,6 +100,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -134,15 +147,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -440,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C9"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -557,9 +576,23 @@
         <v>10007</v>
       </c>
     </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10">
+        <v>123</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B10" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>